<commit_message>
gc_57_11 update (2 to 6)
ear sheet rep 2 to rep 6 added
</commit_message>
<xml_diff>
--- a/data/Grain_Counting/gc_57_11.xlsx
+++ b/data/Grain_Counting/gc_57_11.xlsx
@@ -8,12 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/han-wenhsu/Library/Mobile Documents/com~apple~CloudDocs/HU Dokumente/6. Semester/Studienprojekt/Ear_development_BSC_project_hwh/data/Grain_Counting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E96D21-5300-714B-B33B-995EB7F9C0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE2EB30-618E-A748-B082-F1126D977E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rep1" sheetId="1" r:id="rId1"/>
+    <sheet name="rep2" sheetId="2" r:id="rId2"/>
+    <sheet name="rep3" sheetId="3" r:id="rId3"/>
+    <sheet name="rep4" sheetId="4" r:id="rId4"/>
+    <sheet name="rep5" sheetId="5" r:id="rId5"/>
+    <sheet name="rep6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,8 +29,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B330A87E-C43C-1E45-BCDD-7D1C4B076E21}</author>
+  </authors>
+  <commentList>
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{B330A87E-C43C-1E45-BCDD-7D1C4B076E21}">
+      <text>
+        <t>[對話串註解]
+您的 Excel 版本可讓您讀取此對話串註解; 但若以較新的 Excel 版本開啟此檔案，將會移除對它進行的所有編輯。深入了解: https://go.microsoft.com/fwlink/?linkid=870924。
+註解:
+    fell off</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="18">
   <si>
     <t>var</t>
   </si>
@@ -71,12 +94,30 @@
     <t>1,3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>capone</t>
+  </si>
+  <si>
+    <t>capone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plot_id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,8 +133,29 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft JhengHei UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,8 +174,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -136,13 +210,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -153,6 +262,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -170,6 +303,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Han-Wen Hsu" id="{C402F57F-94CF-2B41-B479-8D9EBB7214BF}" userId="S::Han-Wen.Hsu@cmsa3.onmicrosoft.com::301a0419-fe08-477a-a184-1502ab76c5f9" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,12 +606,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H6" dT="2023-06-22T09:43:16.40" personId="{C402F57F-94CF-2B41-B479-8D9EBB7214BF}" id="{B330A87E-C43C-1E45-BCDD-7D1C4B076E21}">
+    <text>fell off</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -683,6 +830,12 @@
       <c r="F8" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -703,6 +856,12 @@
       <c r="F9" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -723,6 +882,12 @@
       <c r="F10" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -743,6 +908,12 @@
       <c r="F11" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -763,6 +934,9 @@
       <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
       <c r="H12" s="3">
         <v>1</v>
       </c>
@@ -786,6 +960,12 @@
       <c r="F13" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -806,6 +986,9 @@
       <c r="F14" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
       <c r="H14" s="3">
         <v>1</v>
       </c>
@@ -829,6 +1012,9 @@
       <c r="F15" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
       <c r="H15" s="3">
         <v>1</v>
       </c>
@@ -855,6 +1041,9 @@
       <c r="G16" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -875,6 +1064,12 @@
       <c r="F17" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -895,6 +1090,12 @@
       <c r="F18" s="3">
         <v>2</v>
       </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -915,6 +1116,12 @@
       <c r="F19" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -938,6 +1145,9 @@
       <c r="G20" s="3">
         <v>1</v>
       </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -955,6 +1165,12 @@
       <c r="E21" s="2">
         <v>2</v>
       </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
       <c r="H21" s="3">
         <v>1</v>
       </c>
@@ -975,8 +1191,14 @@
       <c r="E22" s="2">
         <v>2</v>
       </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
       <c r="G22" s="3">
         <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -995,7 +1217,2501 @@
       <c r="E23" s="2">
         <v>2</v>
       </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
       <c r="H23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD609FEA-AE2C-1F4E-8053-DF41718EC9A1}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="6" max="8" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>57</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>57</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>57</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1">
+        <v>57</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>57</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>57</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>57</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>57</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1">
+        <v>57</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1">
+        <v>57</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1">
+        <v>57</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387D7DB5-1DD5-7840-895D-92B4B2474471}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="6" max="8" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>57</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>57</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>57</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1">
+        <v>57</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>57</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>57</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>57</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>57</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1">
+        <v>57</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1">
+        <v>57</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1">
+        <v>57</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72716BF8-25F5-044F-9E98-E22D2BDAB850}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="6" max="8" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>57</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>57</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>57</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1">
+        <v>57</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>57</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>57</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>57</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>57</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>57</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384BCB77-193B-6141-9D46-54CDCF1292D8}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="8" width="10.83203125" style="3"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7">
+        <v>57</v>
+      </c>
+      <c r="C2" s="7">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7">
+        <v>57</v>
+      </c>
+      <c r="C3" s="7">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7">
+        <v>57</v>
+      </c>
+      <c r="C4" s="7">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="7">
+        <v>57</v>
+      </c>
+      <c r="C5" s="7">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="7">
+        <v>57</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5</v>
+      </c>
+      <c r="D6" s="9">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7">
+        <v>57</v>
+      </c>
+      <c r="C7" s="7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7">
+        <v>57</v>
+      </c>
+      <c r="C8" s="7">
+        <v>5</v>
+      </c>
+      <c r="D8" s="9">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7">
+        <v>57</v>
+      </c>
+      <c r="C9" s="7">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="7">
+        <v>57</v>
+      </c>
+      <c r="C10" s="7">
+        <v>5</v>
+      </c>
+      <c r="D10" s="9">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7">
+        <v>57</v>
+      </c>
+      <c r="C11" s="7">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="7">
+        <v>57</v>
+      </c>
+      <c r="C12" s="7">
+        <v>5</v>
+      </c>
+      <c r="D12" s="9">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7">
+        <v>57</v>
+      </c>
+      <c r="C13" s="7">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7">
+        <v>57</v>
+      </c>
+      <c r="C14" s="7">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7">
+        <v>57</v>
+      </c>
+      <c r="C15" s="7">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="7">
+        <v>57</v>
+      </c>
+      <c r="C16" s="7">
+        <v>5</v>
+      </c>
+      <c r="D16" s="9">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="7">
+        <v>57</v>
+      </c>
+      <c r="C17" s="7">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="7">
+        <v>57</v>
+      </c>
+      <c r="C18" s="7">
+        <v>5</v>
+      </c>
+      <c r="D18" s="9">
+        <v>17</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="7">
+        <v>57</v>
+      </c>
+      <c r="C19" s="7">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="7">
+        <v>57</v>
+      </c>
+      <c r="C20" s="7">
+        <v>5</v>
+      </c>
+      <c r="D20" s="9">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="7">
+        <v>57</v>
+      </c>
+      <c r="C21" s="7">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="7">
+        <v>57</v>
+      </c>
+      <c r="C22" s="7">
+        <v>5</v>
+      </c>
+      <c r="D22" s="9">
+        <v>21</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A822FB41-F222-9243-8507-9B03A81441E2}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="8" width="10.83203125" style="11"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7">
+        <v>57</v>
+      </c>
+      <c r="C2" s="7">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7">
+        <v>57</v>
+      </c>
+      <c r="C3" s="7">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7">
+        <v>57</v>
+      </c>
+      <c r="C4" s="7">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4</v>
+      </c>
+      <c r="F4" s="11">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="7">
+        <v>57</v>
+      </c>
+      <c r="C5" s="7">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="7">
+        <v>57</v>
+      </c>
+      <c r="C6" s="7">
+        <v>6</v>
+      </c>
+      <c r="D6" s="9">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4</v>
+      </c>
+      <c r="F6" s="11">
+        <v>1</v>
+      </c>
+      <c r="G6" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7">
+        <v>57</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7">
+        <v>57</v>
+      </c>
+      <c r="C8" s="7">
+        <v>6</v>
+      </c>
+      <c r="D8" s="9">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="11">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="7">
+        <v>57</v>
+      </c>
+      <c r="C9" s="7">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="11">
+        <v>3</v>
+      </c>
+      <c r="H9" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="7">
+        <v>57</v>
+      </c>
+      <c r="C10" s="7">
+        <v>6</v>
+      </c>
+      <c r="D10" s="9">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="7">
+        <v>57</v>
+      </c>
+      <c r="C11" s="7">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="11">
+        <v>2</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="7">
+        <v>57</v>
+      </c>
+      <c r="C12" s="7">
+        <v>6</v>
+      </c>
+      <c r="D12" s="9">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7">
+        <v>57</v>
+      </c>
+      <c r="C13" s="7">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11">
+        <v>2</v>
+      </c>
+      <c r="H13" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7">
+        <v>57</v>
+      </c>
+      <c r="C14" s="7">
+        <v>6</v>
+      </c>
+      <c r="D14" s="9">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7">
+        <v>57</v>
+      </c>
+      <c r="C15" s="7">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="F15" s="11">
+        <v>2</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="H15" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="7">
+        <v>57</v>
+      </c>
+      <c r="C16" s="7">
+        <v>6</v>
+      </c>
+      <c r="D16" s="9">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
+      <c r="H16" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="7">
+        <v>57</v>
+      </c>
+      <c r="C17" s="7">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1</v>
+      </c>
+      <c r="G17" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="7">
+        <v>57</v>
+      </c>
+      <c r="C18" s="7">
+        <v>6</v>
+      </c>
+      <c r="D18" s="9">
+        <v>17</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="7">
+        <v>57</v>
+      </c>
+      <c r="C19" s="7">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3</v>
+      </c>
+      <c r="F19" s="11">
+        <v>1</v>
+      </c>
+      <c r="H19" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="7">
+        <v>57</v>
+      </c>
+      <c r="C20" s="7">
+        <v>6</v>
+      </c>
+      <c r="D20" s="9">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3</v>
+      </c>
+      <c r="F20" s="11">
+        <v>1</v>
+      </c>
+      <c r="G20" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="7">
+        <v>57</v>
+      </c>
+      <c r="C21" s="7">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3</v>
+      </c>
+      <c r="F21" s="11">
+        <v>1</v>
+      </c>
+      <c r="H21" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="7">
+        <v>57</v>
+      </c>
+      <c r="C22" s="7">
+        <v>6</v>
+      </c>
+      <c r="D22" s="9">
+        <v>21</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="H22" s="11">
         <v>1</v>
       </c>
     </row>

</xml_diff>